<commit_message>
added sts slowing reason(not complete solution) and started adding ajax notes
</commit_message>
<xml_diff>
--- a/Coding notes to be always referenced by.xlsx
+++ b/Coding notes to be always referenced by.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="application.properties" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="thymeleaf" sheetId="5" r:id="rId5"/>
     <sheet name="mariaDB" sheetId="6" r:id="rId6"/>
     <sheet name="Useful Notes" sheetId="7" r:id="rId7"/>
+    <sheet name="Query" sheetId="8" r:id="rId8"/>
+    <sheet name="Ajax" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="206">
   <si>
     <t>mariaDB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -657,6 +659,195 @@
   </si>
   <si>
     <t>Allows Security to variety users and grants certain access to certain specific user, and creates a temporary id and password to login in!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@ManyToOne</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name="user_id", nullable=false)</t>
+  </si>
+  <si>
+    <t>private Uservo uservo;</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy="uservo", fetch=FetchType.EAGER, cascade=CascadeType.ALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private List&lt;ReviewRegistrationvo&gt; reviewRegistrationList = new ArrayList&lt;ReviewRegistrationvo&gt;(); </t>
+  </si>
+  <si>
+    <t>다대일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일대다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>photoshop --&gt; zeplin for css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">sts running realllly slow, what to do? </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plugins/org.eclipse.equinox.launcher_1.5.400.v20190515-0925.jar</t>
+  </si>
+  <si>
+    <t>C:/Program Files/Java/jdk1.8.0_221/bin/javaw.exe</t>
+  </si>
+  <si>
+    <t>plugins/org.eclipse.equinox.launcher.win32.win32.x86_64_1.1.1000.v20190125-2016</t>
+  </si>
+  <si>
+    <t>org.springframework.boot.ide.branding.sts4</t>
+  </si>
+  <si>
+    <t>openFile</t>
+  </si>
+  <si>
+    <t>-XX:+UseG1GC</t>
+  </si>
+  <si>
+    <t>-XX:+UseStringDeduplication</t>
+  </si>
+  <si>
+    <t>-javaagent:C:\Users\Yoon Taewon\Downloads\spring-tool-suite-4-4.3.1.RELEASE-e4.12.0-win32.win32.x86_64\sts-4.3.1.RELEASE\lombok.jar</t>
+  </si>
+  <si>
+    <t>=-vm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-startup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=--launcher.library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-product</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=--launcher.defaultAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-vmargs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-Dosgi.requiredJavaVersion=1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-Xms512m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-Xmx1024m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=--add-modules=ALL-SYSTEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>original file above</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now changed part below</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-XX:PermSize=128m</t>
+  </si>
+  <si>
+    <t>=-Xmx512m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xms랑 xmx를 똑같으 크기로 설정, 최소 heap메모리랑 최대heap메모리 변경이 없어서 속도 향상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-XX:MaxPermSize=128m</t>
+  </si>
+  <si>
+    <t>-XX:NewSize=128m</t>
+  </si>
+  <si>
+    <t>-XX:MaxNewSize=128m</t>
+  </si>
+  <si>
+    <t>-XX:+AggressiveOpts</t>
+  </si>
+  <si>
+    <t>-XX:-UseConcMarkSweepGC</t>
+  </si>
+  <si>
+    <t>=-Xverify:none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-Xmn256m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=-Xms1024m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prefernce--general--show heap status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>turn off unused project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;a onclick="</t>
+  </si>
+  <si>
+    <t>document.querySelector('article').innerHTML = '&lt;h2&gt;html&lt;/h2&gt;html is cool';&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fetch('/').then(function(response){ </t>
+  </si>
+  <si>
+    <t>document.querySelector('article').innerHTML= text;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">}) </t>
+  </si>
+  <si>
+    <t>response.text().then(function(text){</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function callbackme(){</t>
+  </si>
+  <si>
+    <t>console.log('end');</t>
+  </si>
+  <si>
+    <t>callbackme = function(){</t>
+  </si>
+  <si>
+    <t>====</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fetch('/').then(callbackme);</t>
+  </si>
+  <si>
+    <t>== fetch를 한후에 실행을 끝날때가지 기다리고 callbackme란 function를 실행시킨다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1589,77 +1780,80 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="N11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -1813,6 +2007,49 @@
     <row r="45" spans="1:4">
       <c r="A45" s="6" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>152</v>
+      </c>
+      <c r="H50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="H51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1933,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -2077,7 +2314,9 @@
       </c>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2092,6 +2331,289 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetData>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>